<commit_message>
Change in project name
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Sunil\Sunil\Selenium\SeleniumAutomationFramework\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2A22D9-AF23-46C9-B712-C945BF947CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39548851-2AD4-4240-BCC2-8CE5D25E37C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="4152" windowWidth="17280" windowHeight="8088" xr2:uid="{87C163CD-658B-47DD-BDF5-2E752BD65C89}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{87C163CD-658B-47DD-BDF5-2E752BD65C89}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4696E150-736E-4AD3-BE3E-33FD4F7FD95B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -502,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -537,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3831B5A-570E-47EC-8CC0-84C6885062DA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -612,7 +615,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -632,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
added unimplemeted methods to Listener class
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39548851-2AD4-4240-BCC2-8CE5D25E37C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4515D27-F38D-4A8E-80B4-7C51413434F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{87C163CD-658B-47DD-BDF5-2E752BD65C89}"/>
+    <workbookView xWindow="5220" yWindow="4152" windowWidth="17280" windowHeight="8088" xr2:uid="{87C163CD-658B-47DD-BDF5-2E752BD65C89}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>firefox</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -470,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4696E150-736E-4AD3-BE3E-33FD4F7FD95B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -505,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -540,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3831B5A-570E-47EC-8CC0-84C6885062DA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -615,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -635,7 +632,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
added login test cases (#1)
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4515D27-F38D-4A8E-80B4-7C51413434F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144DB315-A6F5-40C7-A1D6-6C0415C6232A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="4152" windowWidth="17280" windowHeight="8088" xr2:uid="{87C163CD-658B-47DD-BDF5-2E752BD65C89}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>testname</t>
   </si>
@@ -52,27 +52,27 @@
     <t>count</t>
   </si>
   <si>
-    <t>loginLogoutTest</t>
-  </si>
-  <si>
-    <t>newTest</t>
+    <t>verifyThatAdminCanLogInWithValidCredentials</t>
   </si>
   <si>
     <t>To check whether the user can successfully login and logout</t>
   </si>
   <si>
+    <t>verifyThatAdminCannotLogInWithInvalidCredentials</t>
+  </si>
+  <si>
     <t>To check this test is executed</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -82,6 +82,9 @@
     <t>fname</t>
   </si>
   <si>
+    <t>browser</t>
+  </si>
+  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -91,38 +94,26 @@
     <t>amuthan</t>
   </si>
   <si>
-    <t>testing mini bytes</t>
-  </si>
-  <si>
-    <t>subscribe</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>admin12</t>
+  </si>
+  <si>
+    <t>sunil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -464,16 +455,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4696E150-736E-4AD3-BE3E-33FD4F7FD95B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.83984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,21 +490,21 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -522,10 +513,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -534,17 +525,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3831B5A-570E-47EC-8CC0-84C6885062DA}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF392B07-ED60-4B3D-AB46-77E1FA45E324}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -564,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -575,16 +565,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -595,80 +585,59 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added invali cred test case
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144DB315-A6F5-40C7-A1D6-6C0415C6232A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B532B49A-A5CA-4777-A3A8-8FDEFEDA114A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="5556" yWindow="4152" windowWidth="17280" windowHeight="8088" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -100,10 +100,13 @@
     <t>firefox</t>
   </si>
   <si>
-    <t>admin12</t>
-  </si>
-  <si>
     <t>sunil</t>
+  </si>
+  <si>
+    <t>Admin12</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -528,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF392B07-ED60-4B3D-AB46-77E1FA45E324}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -605,13 +608,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -625,13 +628,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Added password only test case
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE391F2-D6D4-49A6-9B98-E99AAE174498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0DECD9-D99F-45B0-8E19-DD89D0C7E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5556" yWindow="4152" windowWidth="17280" windowHeight="8088" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>testname</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>verifyThatAdminCannotLogInWithOnlyPasswordFilled</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -505,7 +511,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -539,9 +545,26 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -552,10 +575,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF392B07-ED60-4B3D-AB46-77E1FA45E324}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -703,6 +726,46 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Page OrangeUpdatePasswordPage, Test OrangeHRMUpdateTest,Change in dta.xlxs
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0DECD9-D99F-45B0-8E19-DD89D0C7E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6DAF13-8FD4-4D94-AF1F-FC9053CDC490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="34">
   <si>
     <t>testname</t>
   </si>
@@ -119,16 +119,40 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>verifyThatUserCanChangePasswordWithValidCredentials</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>currentpassword</t>
+  </si>
+  <si>
+    <t>newpassword</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>admin111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -471,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.9453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -565,6 +589,23 @@
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -575,18 +616,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF392B07-ED60-4B3D-AB46-77E1FA45E324}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.05078125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,8 +649,17 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -625,8 +678,17 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -645,8 +707,17 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -665,8 +736,17 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -685,8 +765,17 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -705,8 +794,17 @@
       <c r="F6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -725,8 +823,17 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -745,8 +852,17 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -765,8 +881,76 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Custom annotaion @Sheet to framwork.
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6DAF13-8FD4-4D94-AF1F-FC9053CDC490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB64D829-EF86-43EC-BE05-A46F2C9E82F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
+    <sheet name="USERACCOUNTMANAGEMENTDATA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="34">
   <si>
     <t>testname</t>
   </si>
@@ -619,7 +620,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -953,4 +954,117 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A0A6CB-F5AE-446B-B73A-0299EFF5044E}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="45.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.62890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.05078125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new test case and also added logic to read  multiple sheets from excel in excelutils
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB64D829-EF86-43EC-BE05-A46F2C9E82F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CDC2AC-62BB-44E9-A067-C9B77E59178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="38">
   <si>
     <t>testname</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>admin111</t>
+  </si>
+  <si>
+    <t>verifyThatUserCannotChangePasswordWithInvalidCurrentPassword</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>admin112</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -496,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -610,6 +622,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -617,10 +646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF392B07-ED60-4B3D-AB46-77E1FA45E324}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -892,64 +921,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -958,15 +929,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A0A6CB-F5AE-446B-B73A-0299EFF5044E}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="45.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.5234375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.62890625" bestFit="1" customWidth="1"/>
@@ -1064,7 +1035,66 @@
         <v>33</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added verifyThatUserCannotChangePasswordWhenTheNewPasswordsDoNotMatch test case under UserAccountManagement.
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CDC2AC-62BB-44E9-A067-C9B77E59178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C0E8A1-2EFC-43EB-8119-CFCE2ED8FAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="41">
   <si>
     <t>testname</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>verifyThatUserCannotChangePasswordWhenTheNewPasswordsDoNotMatch</t>
+  </si>
+  <si>
+    <t>admin132</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -508,15 +517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="54.9453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -636,6 +645,23 @@
         <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -929,10 +955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A0A6CB-F5AE-446B-B73A-0299EFF5044E}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1093,6 +1119,64 @@
         <v>33</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added verifyThatUserCannotChangePasswordWhenThePasswoedDoesNotMeetSpecifiedCriteria test case
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C0E8A1-2EFC-43EB-8119-CFCE2ED8FAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3020828D-C8D7-4AB2-8820-4B6D5BD276F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="44">
   <si>
     <t>testname</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>verifyThatUserCannotChangePasswordWhenThePasswoedDoesNotMeetSpecifiedCriteria</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>admin1</t>
   </si>
 </sst>
 </file>
@@ -517,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="61.734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -662,6 +671,23 @@
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -955,15 +981,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A0A6CB-F5AE-446B-B73A-0299EFF5044E}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="64.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.41796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.62890625" bestFit="1" customWidth="1"/>
@@ -1177,6 +1203,64 @@
         <v>39</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
addedne test case in UsrAccount management test
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3020828D-C8D7-4AB2-8820-4B6D5BD276F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763411CB-07C9-4579-94A8-DD847C8806F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="47">
   <si>
     <t>testname</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>admin1</t>
+  </si>
+  <si>
+    <t>verifyThatUserCannotChangePasswordWhenAllFieldsAreEmpty</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -526,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -688,6 +697,23 @@
         <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -981,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A0A6CB-F5AE-446B-B73A-0299EFF5044E}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1261,6 +1287,64 @@
         <v>39</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new page class, new test for admin user, added new class for uniqueusername, dded class for left Menu component
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B13E4C-3328-4B7D-BBCB-861807C7F706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9878D6-B397-4CEA-A705-BF0E5BA82A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="52">
   <si>
     <t>testname</t>
   </si>
@@ -186,13 +186,13 @@
     <t>employeename</t>
   </si>
   <si>
-    <t>shamsundar</t>
-  </si>
-  <si>
     <t>sham12345</t>
   </si>
   <si>
-    <t>sham</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Orange  Test</t>
   </si>
 </sst>
 </file>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -733,6 +733,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -740,10 +757,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04EA249-C286-437E-A58A-69C4BA98E9D1}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -755,7 +772,7 @@
     <col min="7" max="7" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -775,10 +792,13 @@
         <v>15</v>
       </c>
       <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -786,10 +806,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>51</v>
@@ -798,10 +818,13 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -809,10 +832,10 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>51</v>
@@ -821,7 +844,10 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test case ID 13
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
+++ b/SeleniumAutomationFramework/src/test/resources/Excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrx\git\repository\SeleniumAutomationFramework\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9878D6-B397-4CEA-A705-BF0E5BA82A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D946619-9D50-47A0-BE9A-E0452F39E0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8729CB30-0DA3-4B54-AFF0-045232716AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="54">
   <si>
     <t>testname</t>
   </si>
@@ -192,7 +192,13 @@
     <t>10</t>
   </si>
   <si>
-    <t>Orange  Test</t>
+    <t>verifyThaTheNumberOfUserRecordsIncreasesAfterAddingANewUser</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Orange Middle NameMiddle Name Test</t>
   </si>
 </sst>
 </file>
@@ -551,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63E9A7D-678B-40CF-9D0A-F339110468CD}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -750,6 +756,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -757,19 +780,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04EA249-C286-437E-A58A-69C4BA98E9D1}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="33.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.7890625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.9453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -812,7 +835,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -838,7 +861,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -847,6 +870,58 @@
         <v>49</v>
       </c>
       <c r="H3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>